<commit_message>
DCU wiring spreadsheet updated with new connections for (unlatched) START, crash switch, inhibit traction, brake switch, temp gauge, fuel gauge and alternator warning light.
</commit_message>
<xml_diff>
--- a/master/tritium/DCU wiring.xlsx
+++ b/master/tritium/DCU wiring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="247">
   <si>
     <t>1A</t>
   </si>
@@ -240,9 +240,6 @@
     <t>LGN-WHT</t>
   </si>
   <si>
-    <t>RED-BLU</t>
-  </si>
-  <si>
     <t>RED-GRN</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
     <t>Ignition switch, Igniter, ignition coil</t>
   </si>
   <si>
-    <t>Circuit opening relay coil (controls fuel pump), ST SIGN fuse</t>
-  </si>
-  <si>
     <t>Circuit opening relay, Fuel tank unit</t>
   </si>
   <si>
@@ -363,9 +357,6 @@
     <t>Fuel injectors</t>
   </si>
   <si>
-    <t>Idle speed control solenoid valve</t>
-  </si>
-  <si>
     <t>Purge solenoid valve</t>
   </si>
   <si>
@@ -465,9 +456,6 @@
     <t>WHT 2</t>
   </si>
   <si>
-    <t>RED 2</t>
-  </si>
-  <si>
     <t>RED 3</t>
   </si>
   <si>
@@ -504,12 +492,6 @@
     <t>YEL-BLK 2</t>
   </si>
   <si>
-    <t>Joins YEL-BLK 2 under steering column</t>
-  </si>
-  <si>
-    <t>IGN_START, Latched start, Joins LGN unde steering column</t>
-  </si>
-  <si>
     <t>A24</t>
   </si>
   <si>
@@ -528,42 +510,15 @@
     <t>A13</t>
   </si>
   <si>
-    <t>Join to B32, IGN_ACC, Allow full regen</t>
-  </si>
-  <si>
-    <t>Join to A24, LED Gear 4, Non-pedal DCU presence</t>
-  </si>
-  <si>
-    <t>Join to B13, Brakelight input, Inhibit traction</t>
-  </si>
-  <si>
-    <t>Join to A13, Brakelight input, request brakelight</t>
-  </si>
-  <si>
-    <t>Join to A7, LED Gear 3, Charge A mode</t>
-  </si>
-  <si>
-    <t>Join to B7, LED Gear 3, Charge B mode</t>
-  </si>
-  <si>
     <t>A6</t>
   </si>
   <si>
     <t>B6</t>
   </si>
   <si>
-    <t>A27</t>
-  </si>
-  <si>
-    <t>B27</t>
-  </si>
-  <si>
     <t>IGN_RUN, Crash switch COM</t>
   </si>
   <si>
-    <t xml:space="preserve">Diode inserted at Cct opening relay and </t>
-  </si>
-  <si>
     <t>A_BRAKELIGHT</t>
   </si>
   <si>
@@ -624,13 +579,163 @@
     <t>YEL 2</t>
   </si>
   <si>
-    <t>Fuel tank unit, Fuel gauge</t>
-  </si>
-  <si>
     <t>Gauge1, Tacho, Joins YEL-BLU 2 in 12V box to reach tacho</t>
   </si>
   <si>
     <t>A Battery contactors (rear), Disconnect from WHT-RED at Cct opening relay and connect to BRN-YEL or WHT-GRN</t>
+  </si>
+  <si>
+    <t>ECU pin</t>
+  </si>
+  <si>
+    <t>GND for Throttle, Airflow, Coolant thermo, Crank angle, O2 sensors</t>
+  </si>
+  <si>
+    <t>BLU-ORG 2</t>
+  </si>
+  <si>
+    <t>ORG</t>
+  </si>
+  <si>
+    <t>WHT 3</t>
+  </si>
+  <si>
+    <t>BRN 2</t>
+  </si>
+  <si>
+    <t>Crash switch NC, Joins WHT 3 at ECU/DCU location</t>
+  </si>
+  <si>
+    <t>Crash switch</t>
+  </si>
+  <si>
+    <t>Crash switch NC, Joins WHT-RED at ECU/DCU location</t>
+  </si>
+  <si>
+    <t>Fuel door, Charge cable A</t>
+  </si>
+  <si>
+    <t>Fuel door, Charge cable B</t>
+  </si>
+  <si>
+    <t>RED 4</t>
+  </si>
+  <si>
+    <t>BLU 2</t>
+  </si>
+  <si>
+    <t>GRN 2</t>
+  </si>
+  <si>
+    <t>Heater control unit (switched to GND when fan on)</t>
+  </si>
+  <si>
+    <t>YEL-RED 2</t>
+  </si>
+  <si>
+    <t>A36</t>
+  </si>
+  <si>
+    <t>Doesn't exist on our model</t>
+  </si>
+  <si>
+    <t>IGN_START</t>
+  </si>
+  <si>
+    <t>Brakelight input</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>BLU-ORG-SLV</t>
+  </si>
+  <si>
+    <t>BLU-ORG 3</t>
+  </si>
+  <si>
+    <t>A37</t>
+  </si>
+  <si>
+    <t>Heater relay on heater cover to Heater contactors, 12V box</t>
+  </si>
+  <si>
+    <t>Heater microsw inserted in this wire between heater unit and relay on heater cover whose contact drives BLU-ORG 3</t>
+  </si>
+  <si>
+    <t>Idle speed control solenoid valve (cut under dash)</t>
+  </si>
+  <si>
+    <t>Stress level gauge (pressure gauge), Gauge2, Joined to YEL-RED2 under dash</t>
+  </si>
+  <si>
+    <t>LED_FAULT_1, joined to WHT-BLK under dash, Alternator light (Inst cluster)</t>
+  </si>
+  <si>
+    <t>Not used. May be the one that's cut under dash. See BLU-ORG-SLV</t>
+  </si>
+  <si>
+    <t>Fan switch. Switched to GND when fan on speed 2 or more</t>
+  </si>
+  <si>
+    <t>Doesn't exist in our model</t>
+  </si>
+  <si>
+    <t>A28</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>Gear 2, Crash switch NO</t>
+  </si>
+  <si>
+    <t>Oil pressure gauge to oil pres sensor, Joined to YEL-RED under dash</t>
+  </si>
+  <si>
+    <t>Oil Pressure</t>
+  </si>
+  <si>
+    <t>Joined to B32, IGN_ACC, Allow full regen</t>
+  </si>
+  <si>
+    <t>Joined to A24, LED Gear 4, Non-pedal DCU presence</t>
+  </si>
+  <si>
+    <t>Joined to B13, Gear 3 input, Inhibit traction</t>
+  </si>
+  <si>
+    <t>Joined to A7, LED Gear 3, Charge A mode</t>
+  </si>
+  <si>
+    <t>Joined to A13, Brakelight input, request brakelight</t>
+  </si>
+  <si>
+    <t>Joined to B7, LED Gear 3, Charge B mode</t>
+  </si>
+  <si>
+    <t>RED 2 (coax)</t>
+  </si>
+  <si>
+    <t>RED-BLU (coax)</t>
+  </si>
+  <si>
+    <t>Airflow meter (not in 12V box, prob near diag conn)</t>
+  </si>
+  <si>
+    <t>Carries TRACTION signal to Pumps relay in 12V box, Joins LGN under dash</t>
+  </si>
+  <si>
+    <t>YEL 3</t>
+  </si>
+  <si>
+    <t>Joins YEL-BLK 2 under dash</t>
+  </si>
+  <si>
+    <t>Connected to Fuel gauge YEL 3 under dash, Gauge4</t>
+  </si>
+  <si>
+    <t>Fuel tank unit, Fuel gauge (cut under dash)</t>
   </si>
   <si>
     <r>
@@ -652,81 +757,33 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Battery contactors (rear), Cut wire under steering wheel and connect to BRN or LGN-YEL</t>
+      <t xml:space="preserve"> Battery contactors (rear), connected to BRN or LGN-YEL under dash</t>
     </r>
   </si>
   <si>
-    <t>ECU pin</t>
-  </si>
-  <si>
-    <t>GND for Throttle, Airflow, Coolant thermo, Crank angle, O2 sensors</t>
-  </si>
-  <si>
-    <t>BLU-ORG 2</t>
-  </si>
-  <si>
-    <t>ORG</t>
-  </si>
-  <si>
-    <t>WHT 3</t>
-  </si>
-  <si>
-    <t>BRN 2</t>
-  </si>
-  <si>
-    <t>Crash switch NC, Joins WHT 3 at ECU/DCU location</t>
-  </si>
-  <si>
-    <t>Crash switch</t>
-  </si>
-  <si>
-    <t>Gear 1, Crash switch NO</t>
-  </si>
-  <si>
-    <t>Crash switch NC, Joins WHT-RED at ECU/DCU location</t>
-  </si>
-  <si>
-    <t>Fuel door, Charge cable A</t>
-  </si>
-  <si>
-    <t>Fuel door, Charge cable B</t>
-  </si>
-  <si>
-    <t>RED 4</t>
-  </si>
-  <si>
-    <t>BLU 2</t>
-  </si>
-  <si>
-    <t>GRN 2</t>
-  </si>
-  <si>
-    <t>Heater control unit (switched to GND when fan on)</t>
-  </si>
-  <si>
-    <t>Insert heater usw in this wire between heater unit and relay near DCUs whose contact drives BLU-YEL</t>
-  </si>
-  <si>
-    <t>YEL-RED 2</t>
-  </si>
-  <si>
-    <t>A36</t>
-  </si>
-  <si>
-    <t>Stress level gauge (pressure gauge), Join to YEL-RED2 in 12V box</t>
-  </si>
-  <si>
-    <t>Oil pressure gauge, Inst clstr 2B, to oil pres sensor, Join to YEL-RED in 12V box</t>
-  </si>
-  <si>
-    <t>Heater relay near DCUs to Heater contactors, 12V box</t>
+    <t>Fuel gauge, connected to BLU-ORG 2 under dash</t>
+  </si>
+  <si>
+    <t>Temp gauge</t>
+  </si>
+  <si>
+    <t>BLK-BLU 2</t>
+  </si>
+  <si>
+    <t>Gauge 3 (temp) , connected to BLK-BLU 2 in 12V box.</t>
+  </si>
+  <si>
+    <t>Temp gauge connected to BLU-WHT in 12V box</t>
+  </si>
+  <si>
+    <t>Circuit opening relay coil (controls fuel pump), ST SIGN fuse from key START via Transmission starter interlock switch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,6 +871,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFE7E200"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -937,7 +1001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1002,6 +1066,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1301,17 +1366,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R77"/>
+  <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="750"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="750" topLeftCell="A28" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.42578125" style="46" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="49.5703125" style="46" customWidth="1"/>
     <col min="6" max="17" width="5.7109375" customWidth="1"/>
@@ -1320,75 +1385,75 @@
   <sheetData>
     <row r="1" spans="1:18" s="46" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="M1" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="N1" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="O1" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="P1" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="46" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="46" t="s">
-        <v>206</v>
-      </c>
-      <c r="G1" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="I1" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="J1" s="46" t="s">
-        <v>140</v>
-      </c>
-      <c r="K1" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="N1" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="O1" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="P1" s="46" t="s">
-        <v>141</v>
-      </c>
       <c r="Q1" s="46" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="R1" s="46" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="46" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1396,148 +1461,154 @@
     </row>
     <row r="3" spans="1:18" ht="30">
       <c r="A3" s="50" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="30">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="45">
       <c r="A4" s="46" t="s">
-        <v>100</v>
+        <v>246</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>156</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>206</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>117</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1548,16 +1619,16 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -1565,22 +1636,22 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1597,53 +1668,62 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
       </c>
       <c r="O15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>208</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" ht="30">
       <c r="A17" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="D17" t="s">
+        <v>209</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -1651,16 +1731,16 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -1668,13 +1748,13 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -1682,16 +1762,16 @@
     </row>
     <row r="20" spans="1:16" ht="30">
       <c r="A20" s="46" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
@@ -1705,13 +1785,13 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
         <v>57</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
@@ -1719,36 +1799,36 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
         <v>58</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="F23" t="s">
         <v>21</v>
       </c>
       <c r="P23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
         <v>64</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
@@ -1756,13 +1836,13 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
         <v>64</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
         <v>23</v>
@@ -1770,77 +1850,77 @@
     </row>
     <row r="26" spans="1:16" ht="30">
       <c r="A26" s="46" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="B26" t="s">
         <v>65</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F26" t="s">
         <v>24</v>
       </c>
       <c r="M26" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N26" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="O26" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="30">
       <c r="A27" s="46" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F27" t="s">
         <v>25</v>
       </c>
       <c r="M27" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N27" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="O27" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="E28" s="46" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="F28" t="s">
         <v>26</v>
       </c>
       <c r="N28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1851,36 +1931,39 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
         <v>69</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="E30" s="46" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="F30" t="s">
         <v>28</v>
       </c>
       <c r="N30" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="E31" s="46" t="s">
+        <v>220</v>
       </c>
       <c r="F31" t="s">
         <v>29</v>
@@ -1888,25 +1971,25 @@
     </row>
     <row r="32" spans="1:16" ht="30">
       <c r="A32" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="F32" t="s">
         <v>30</v>
       </c>
       <c r="I32" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -1917,53 +2000,53 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
         <v>72</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F34" t="s">
         <v>32</v>
       </c>
       <c r="M34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
         <v>73</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="F35" t="s">
         <v>33</v>
       </c>
       <c r="O35" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F36" t="s">
         <v>34</v>
@@ -1971,61 +2054,64 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="46" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>233</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" ht="30">
       <c r="A38" s="46" t="s">
-        <v>111</v>
+        <v>234</v>
       </c>
       <c r="B38" t="s">
-        <v>149</v>
+        <v>232</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F38" t="s">
         <v>36</v>
       </c>
       <c r="M38" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="46" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F39" t="s">
         <v>37</v>
       </c>
       <c r="M39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="E40" s="46" t="s">
+        <v>244</v>
       </c>
       <c r="F40" t="s">
         <v>38</v>
@@ -2051,16 +2137,16 @@
     </row>
     <row r="44" spans="1:15" ht="30">
       <c r="A44" s="46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="F44" t="s">
         <v>42</v>
@@ -2068,33 +2154,39 @@
     </row>
     <row r="45" spans="1:15" ht="30">
       <c r="A45" s="46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>163</v>
+        <v>235</v>
       </c>
       <c r="F45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" ht="30">
       <c r="A46" s="46" t="s">
-        <v>115</v>
+        <v>215</v>
       </c>
       <c r="B46" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="D46" t="s">
+        <v>212</v>
+      </c>
+      <c r="E46" s="46" t="s">
+        <v>238</v>
       </c>
       <c r="F46" t="s">
         <v>60</v>
@@ -2102,118 +2194,117 @@
     </row>
     <row r="47" spans="1:15" ht="30">
       <c r="A47" s="46" t="s">
-        <v>116</v>
+        <v>215</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" t="s">
-        <v>224</v>
+        <v>211</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="F47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="30">
+      <c r="A48" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48" t="s">
+        <v>205</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="F48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
-      <c r="C48" s="37"/>
-      <c r="F48" t="s">
+    <row r="49" spans="1:17">
+      <c r="C49" s="37"/>
+      <c r="F49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
-      <c r="A49" s="51"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="F49" t="s">
+    <row r="50" spans="1:17">
+      <c r="A50" s="51"/>
+      <c r="B50" s="48"/>
+      <c r="C50" s="48"/>
+      <c r="F50" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:17">
-      <c r="A51" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" t="s">
-        <v>152</v>
-      </c>
-      <c r="C51" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="L51" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17">
+      <c r="A51" s="51"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="48"/>
+    </row>
+    <row r="52" spans="1:17" ht="45">
       <c r="A52" s="46" t="s">
-        <v>97</v>
+        <v>219</v>
       </c>
       <c r="B52" t="s">
-        <v>144</v>
-      </c>
-      <c r="C52" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="L52" t="s">
-        <v>117</v>
+        <v>210</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="46" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" s="46" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="I53" t="s">
-        <v>125</v>
-      </c>
-      <c r="J53" t="s">
-        <v>117</v>
+        <v>148</v>
+      </c>
+      <c r="C53" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="L53" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:17">
       <c r="A54" s="46" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>148</v>
-      </c>
-      <c r="C54" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="I54" t="s">
-        <v>122</v>
-      </c>
-      <c r="J54" t="s">
-        <v>117</v>
+        <v>141</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="L54" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:17">
       <c r="A55" s="46" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B55" t="s">
-        <v>98</v>
-      </c>
-      <c r="C55" s="43" t="s">
-        <v>80</v>
+        <v>146</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="I55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J55" t="s">
-        <v>117</v>
-      </c>
-      <c r="P55" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:17">
@@ -2221,327 +2312,405 @@
         <v>105</v>
       </c>
       <c r="B56" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="I56" t="s">
+        <v>119</v>
+      </c>
+      <c r="J56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="I57" t="s">
+        <v>120</v>
+      </c>
+      <c r="J57" t="s">
+        <v>114</v>
+      </c>
+      <c r="P57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="A58" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="G58" t="s">
+        <v>114</v>
+      </c>
+      <c r="H58" t="s">
+        <v>7</v>
+      </c>
+      <c r="I58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="45">
+      <c r="A59" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E56" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="G56" t="s">
-        <v>117</v>
-      </c>
-      <c r="H56" t="s">
-        <v>117</v>
-      </c>
-      <c r="I56" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" ht="45">
-      <c r="A57" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" t="s">
-        <v>151</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E57" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="K57" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" ht="30">
-      <c r="A58" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="B58" t="s">
-        <v>79</v>
-      </c>
-      <c r="C58" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="E58" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="G58" t="s">
-        <v>117</v>
-      </c>
-      <c r="K58" t="s">
-        <v>117</v>
-      </c>
-      <c r="M58" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17">
-      <c r="A59" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="B59" t="s">
-        <v>102</v>
-      </c>
-      <c r="C59" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="G59" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17">
+      <c r="C59" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E59" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="K59" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="30">
       <c r="A60" s="46" t="s">
         <v>104</v>
       </c>
       <c r="B60" t="s">
-        <v>153</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E60" s="46" t="s">
+        <v>237</v>
       </c>
       <c r="G60" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" ht="30">
+        <v>114</v>
+      </c>
+      <c r="K60" t="s">
+        <v>114</v>
+      </c>
+      <c r="M60" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17">
       <c r="A61" s="46" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="45" t="s">
-        <v>80</v>
+        <v>100</v>
+      </c>
+      <c r="C61" s="44" t="s">
+        <v>79</v>
       </c>
       <c r="G61" t="s">
-        <v>117</v>
-      </c>
-      <c r="I61" t="s">
-        <v>126</v>
-      </c>
-      <c r="K61" t="s">
-        <v>117</v>
-      </c>
-      <c r="L61" t="s">
-        <v>117</v>
-      </c>
-      <c r="M61" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:17">
       <c r="A62" s="46" t="s">
-        <v>141</v>
+        <v>102</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
-      </c>
-      <c r="C62" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="P62" t="s">
-        <v>117</v>
+        <v>149</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G62" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="30">
       <c r="A63" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="G63" t="s">
+        <v>114</v>
+      </c>
+      <c r="I63" t="s">
+        <v>123</v>
+      </c>
+      <c r="K63" t="s">
+        <v>114</v>
+      </c>
+      <c r="L63" t="s">
+        <v>114</v>
+      </c>
+      <c r="M63" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="A64" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="B64" t="s">
+        <v>139</v>
+      </c>
+      <c r="C64" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="P64" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" ht="30">
+      <c r="A65" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="B65" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" s="33"/>
+      <c r="E65" s="46" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
+      <c r="A66" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="B66" t="s">
+        <v>236</v>
+      </c>
+      <c r="C66" s="33"/>
+      <c r="E66" s="46" t="s">
+        <v>241</v>
+      </c>
+      <c r="H66" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" ht="30">
+      <c r="A67" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="B67" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E67" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="H67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
+      <c r="A68" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="B68" t="s">
+        <v>243</v>
+      </c>
+      <c r="C68" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="E68" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="H68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
+      <c r="D69" t="s">
+        <v>154</v>
+      </c>
+      <c r="E69" s="46" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
+      <c r="D70" t="s">
+        <v>155</v>
+      </c>
+      <c r="E70" s="46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18">
+      <c r="B71" t="s">
+        <v>200</v>
+      </c>
+      <c r="C71" s="55"/>
+      <c r="D71" t="s">
+        <v>158</v>
+      </c>
+      <c r="E71" s="46" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
+      <c r="B72" t="s">
+        <v>200</v>
+      </c>
+      <c r="C72" s="55"/>
+      <c r="D72" t="s">
+        <v>159</v>
+      </c>
+      <c r="E72" s="46" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18">
+      <c r="B73" t="s">
+        <v>201</v>
+      </c>
+      <c r="C73" s="56"/>
+      <c r="D73" t="s">
+        <v>221</v>
+      </c>
+      <c r="E73" s="46" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18">
+      <c r="B74" t="s">
+        <v>201</v>
+      </c>
+      <c r="C74" s="56"/>
+      <c r="D74" t="s">
+        <v>161</v>
+      </c>
+      <c r="E74" s="46" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18">
+      <c r="B75" t="s">
         <v>202</v>
       </c>
-      <c r="B63" t="s">
-        <v>201</v>
-      </c>
-      <c r="C63" s="33"/>
-      <c r="E63" s="46" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" ht="30">
-      <c r="B64" t="s">
+      <c r="C75" s="57"/>
+      <c r="D75" t="s">
+        <v>162</v>
+      </c>
+      <c r="E75" s="46" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
+      <c r="B76" t="s">
+        <v>202</v>
+      </c>
+      <c r="C76" s="57"/>
+      <c r="D76" t="s">
+        <v>163</v>
+      </c>
+      <c r="E76" s="46" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18">
+      <c r="B77" t="s">
+        <v>194</v>
+      </c>
+      <c r="C77" s="52"/>
+      <c r="D77" t="s">
+        <v>164</v>
+      </c>
+      <c r="E77" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="R77" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18">
+      <c r="B78" t="s">
+        <v>194</v>
+      </c>
+      <c r="C78" s="52"/>
+      <c r="D78" t="s">
+        <v>165</v>
+      </c>
+      <c r="E78" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="R78" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18">
+      <c r="B79" t="s">
+        <v>192</v>
+      </c>
+      <c r="C79" s="53"/>
+      <c r="D79" t="s">
+        <v>222</v>
+      </c>
+      <c r="E79" s="46" t="s">
         <v>223</v>
       </c>
-      <c r="C64" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="E64" s="46" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="65" spans="2:18">
-      <c r="D65" t="s">
-        <v>158</v>
-      </c>
-      <c r="E65" s="46" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="66" spans="2:18">
-      <c r="D66" t="s">
-        <v>159</v>
-      </c>
-      <c r="E66" s="46" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="67" spans="2:18">
-      <c r="B67" t="s">
-        <v>218</v>
-      </c>
-      <c r="C67" s="55"/>
-      <c r="D67" t="s">
-        <v>164</v>
-      </c>
-      <c r="E67" s="46" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="68" spans="2:18">
-      <c r="B68" t="s">
-        <v>218</v>
-      </c>
-      <c r="C68" s="55"/>
-      <c r="D68" t="s">
-        <v>165</v>
-      </c>
-      <c r="E68" s="46" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="69" spans="2:18">
-      <c r="B69" t="s">
-        <v>219</v>
-      </c>
-      <c r="C69" s="56"/>
-      <c r="D69" t="s">
-        <v>166</v>
-      </c>
-      <c r="E69" s="46" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="70" spans="2:18">
-      <c r="B70" t="s">
-        <v>219</v>
-      </c>
-      <c r="C70" s="56"/>
-      <c r="D70" t="s">
-        <v>167</v>
-      </c>
-      <c r="E70" s="46" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="71" spans="2:18">
-      <c r="B71" t="s">
-        <v>220</v>
-      </c>
-      <c r="C71" s="57"/>
-      <c r="D71" t="s">
-        <v>168</v>
-      </c>
-      <c r="E71" s="46" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="72" spans="2:18">
-      <c r="B72" t="s">
-        <v>220</v>
-      </c>
-      <c r="C72" s="57"/>
-      <c r="D72" t="s">
-        <v>169</v>
-      </c>
-      <c r="E72" s="46" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="73" spans="2:18">
-      <c r="B73" t="s">
-        <v>211</v>
-      </c>
-      <c r="C73" s="52"/>
-      <c r="D73" t="s">
-        <v>176</v>
-      </c>
-      <c r="E73" s="46" t="s">
-        <v>180</v>
-      </c>
-      <c r="R73" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="74" spans="2:18">
-      <c r="B74" t="s">
-        <v>211</v>
-      </c>
-      <c r="C74" s="52"/>
-      <c r="D74" t="s">
-        <v>177</v>
-      </c>
-      <c r="E74" s="46" t="s">
-        <v>180</v>
-      </c>
-      <c r="R74" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="75" spans="2:18">
-      <c r="B75" t="s">
-        <v>209</v>
-      </c>
-      <c r="C75" s="53"/>
-      <c r="D75" t="s">
-        <v>178</v>
-      </c>
-      <c r="E75" s="46" t="s">
-        <v>214</v>
-      </c>
-      <c r="R75" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="76" spans="2:18">
-      <c r="B76" t="s">
-        <v>209</v>
-      </c>
-      <c r="C76" s="53"/>
-      <c r="D76" t="s">
-        <v>179</v>
-      </c>
-      <c r="E76" s="46" t="s">
-        <v>214</v>
-      </c>
-      <c r="R76" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="77" spans="2:18">
-      <c r="B77" t="s">
-        <v>210</v>
-      </c>
-      <c r="C77" s="54"/>
-      <c r="E77" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="R77" t="s">
-        <v>117</v>
+      <c r="R79" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18">
+      <c r="B80" t="s">
+        <v>192</v>
+      </c>
+      <c r="C80" s="53"/>
+      <c r="D80" t="s">
+        <v>222</v>
+      </c>
+      <c r="E80" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="R80" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="2:18">
+      <c r="B81" t="s">
+        <v>193</v>
+      </c>
+      <c r="C81" s="54"/>
+      <c r="E81" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="R81" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Deleted second "A25" DCU pin designation and corrected some descriptions of wires between DCUs, in DCU wiring spreadsheet.
</commit_message>
<xml_diff>
--- a/master/tritium/DCU wiring.xlsx
+++ b/master/tritium/DCU wiring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="248">
   <si>
     <t>1A</t>
   </si>
@@ -411,9 +411,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Crank sensor</t>
   </si>
   <si>
@@ -426,9 +423,6 @@
     <t>DCU pin</t>
   </si>
   <si>
-    <t>DCU description</t>
-  </si>
-  <si>
     <t>Ignit coil</t>
   </si>
   <si>
@@ -582,9 +576,6 @@
     <t>Gauge1, Tacho, Joins YEL-BLU 2 in 12V box to reach tacho</t>
   </si>
   <si>
-    <t>A Battery contactors (rear), Disconnect from WHT-RED at Cct opening relay and connect to BRN-YEL or WHT-GRN</t>
-  </si>
-  <si>
     <t>ECU pin</t>
   </si>
   <si>
@@ -612,12 +603,6 @@
     <t>Crash switch NC, Joins WHT-RED at ECU/DCU location</t>
   </si>
   <si>
-    <t>Fuel door, Charge cable A</t>
-  </si>
-  <si>
-    <t>Fuel door, Charge cable B</t>
-  </si>
-  <si>
     <t>RED 4</t>
   </si>
   <si>
@@ -690,28 +675,7 @@
     <t>Gear 2, Crash switch NO</t>
   </si>
   <si>
-    <t>Oil pressure gauge to oil pres sensor, Joined to YEL-RED under dash</t>
-  </si>
-  <si>
     <t>Oil Pressure</t>
-  </si>
-  <si>
-    <t>Joined to B32, IGN_ACC, Allow full regen</t>
-  </si>
-  <si>
-    <t>Joined to A24, LED Gear 4, Non-pedal DCU presence</t>
-  </si>
-  <si>
-    <t>Joined to B13, Gear 3 input, Inhibit traction</t>
-  </si>
-  <si>
-    <t>Joined to A7, LED Gear 3, Charge A mode</t>
-  </si>
-  <si>
-    <t>Joined to A13, Brakelight input, request brakelight</t>
-  </si>
-  <si>
-    <t>Joined to B7, LED Gear 3, Charge B mode</t>
   </si>
   <si>
     <t>RED 2 (coax)</t>
@@ -777,6 +741,45 @@
   </si>
   <si>
     <t>Circuit opening relay coil (controls fuel pump), ST SIGN fuse from key START via Transmission starter interlock switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGN_ACC, Allow full regen in, joined to B32, </t>
+  </si>
+  <si>
+    <t>LED Gear 4, Non-pedal DCU presence out, joined to A24</t>
+  </si>
+  <si>
+    <t>Gear 3 input, Inhibit traction in, joined to B13</t>
+  </si>
+  <si>
+    <t>LED Gear 3, DCU-B in charge mode out, joined to A7</t>
+  </si>
+  <si>
+    <t>Brakelight input, request brakelight in, joined to A13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED Gear 3, Request brakelight out, joined to B7, </t>
+  </si>
+  <si>
+    <t>EV / DCU description</t>
+  </si>
+  <si>
+    <t>ICE / ECU Description</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>A Battery contactors (rear), joined to BRN-YEL or WHT-GRN under dash</t>
+  </si>
+  <si>
+    <t>Oil pressure gauge to oil pressure sensor, Joined to YEL-RED under dash</t>
+  </si>
+  <si>
+    <t>Fuel door, Charge cable A detect</t>
+  </si>
+  <si>
+    <t>Fuel door, Charge cable B detect</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1372,9 @@
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="750" topLeftCell="A28" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <pane ySplit="750" activePane="bottomLeft"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1385,7 +1389,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="46" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>131</v>
+        <v>242</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>129</v>
@@ -1394,13 +1398,13 @@
         <v>130</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>136</v>
+        <v>241</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G1" s="46" t="s">
         <v>115</v>
@@ -1412,7 +1416,7 @@
         <v>83</v>
       </c>
       <c r="J1" s="46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K1" s="46" t="s">
         <v>127</v>
@@ -1424,24 +1428,24 @@
         <v>109</v>
       </c>
       <c r="N1" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="O1" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="O1" s="46" t="s">
-        <v>133</v>
-      </c>
       <c r="P1" s="46" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Q1" s="46" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R1" s="46" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
@@ -1450,10 +1454,10 @@
         <v>79</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1470,7 +1474,7 @@
         <v>79</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -1487,7 +1491,7 @@
     </row>
     <row r="4" spans="1:18" ht="45">
       <c r="A4" s="46" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
@@ -1496,10 +1500,10 @@
         <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
@@ -1519,7 +1523,7 @@
         <v>79</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -1539,7 +1543,7 @@
         <v>79</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -1559,10 +1563,10 @@
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
@@ -1582,7 +1586,7 @@
         <v>79</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -1602,7 +1606,7 @@
         <v>79</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -1628,7 +1632,7 @@
         <v>79</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -1645,7 +1649,7 @@
         <v>79</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -1677,10 +1681,10 @@
         <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
@@ -1700,10 +1704,10 @@
         <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -1720,10 +1724,10 @@
         <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -1740,7 +1744,7 @@
         <v>79</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -1762,7 +1766,7 @@
     </row>
     <row r="20" spans="1:16" ht="30">
       <c r="A20" s="46" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
@@ -1771,7 +1775,7 @@
         <v>79</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
@@ -1808,10 +1812,10 @@
         <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F23" t="s">
         <v>21</v>
@@ -1850,7 +1854,7 @@
     </row>
     <row r="26" spans="1:16" ht="30">
       <c r="A26" s="46" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B26" t="s">
         <v>65</v>
@@ -1859,7 +1863,7 @@
         <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F26" t="s">
         <v>24</v>
@@ -1876,7 +1880,7 @@
     </row>
     <row r="27" spans="1:16" ht="30">
       <c r="A27" s="46" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
@@ -1885,7 +1889,7 @@
         <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F27" t="s">
         <v>25</v>
@@ -1911,10 +1915,10 @@
         <v>79</v>
       </c>
       <c r="D28" t="s">
+        <v>168</v>
+      </c>
+      <c r="E28" s="46" t="s">
         <v>170</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>172</v>
       </c>
       <c r="F28" t="s">
         <v>26</v>
@@ -1940,10 +1944,10 @@
         <v>79</v>
       </c>
       <c r="D30" t="s">
+        <v>169</v>
+      </c>
+      <c r="E30" s="46" t="s">
         <v>171</v>
-      </c>
-      <c r="E30" s="46" t="s">
-        <v>173</v>
       </c>
       <c r="F30" t="s">
         <v>28</v>
@@ -1963,7 +1967,7 @@
         <v>79</v>
       </c>
       <c r="E31" s="46" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F31" t="s">
         <v>29</v>
@@ -1980,10 +1984,10 @@
         <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F32" t="s">
         <v>30</v>
@@ -2026,10 +2030,10 @@
         <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F35" t="s">
         <v>33</v>
@@ -2057,7 +2061,7 @@
         <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="C37" s="29" t="s">
         <v>79</v>
@@ -2068,10 +2072,10 @@
     </row>
     <row r="38" spans="1:15" ht="30">
       <c r="A38" s="46" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B38" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>79</v>
@@ -2111,7 +2115,7 @@
         <v>79</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="F40" t="s">
         <v>38</v>
@@ -2146,7 +2150,7 @@
         <v>79</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F44" t="s">
         <v>42</v>
@@ -2157,16 +2161,13 @@
         <v>112</v>
       </c>
       <c r="B45" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D45" t="s">
-        <v>156</v>
-      </c>
       <c r="E45" s="46" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="F45" t="s">
         <v>43</v>
@@ -2174,19 +2175,19 @@
     </row>
     <row r="46" spans="1:15" ht="30">
       <c r="A46" s="46" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B46" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="F46" t="s">
         <v>60</v>
@@ -2194,16 +2195,16 @@
     </row>
     <row r="47" spans="1:15" ht="30">
       <c r="A47" s="46" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B47" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>79</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F47" t="s">
         <v>60</v>
@@ -2220,10 +2221,10 @@
         <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F48" t="s">
         <v>61</v>
@@ -2250,16 +2251,16 @@
     </row>
     <row r="52" spans="1:17" ht="45">
       <c r="A52" s="46" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B52" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>79</v>
       </c>
       <c r="E52" s="46" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -2267,7 +2268,7 @@
         <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C53" s="41" t="s">
         <v>79</v>
@@ -2281,7 +2282,7 @@
         <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C54" s="25" t="s">
         <v>79</v>
@@ -2295,7 +2296,7 @@
         <v>105</v>
       </c>
       <c r="B55" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>79</v>
@@ -2312,7 +2313,7 @@
         <v>105</v>
       </c>
       <c r="B56" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C56" s="42" t="s">
         <v>79</v>
@@ -2349,13 +2350,13 @@
         <v>103</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>79</v>
       </c>
       <c r="E58" s="46" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G58" t="s">
         <v>114</v>
@@ -2367,18 +2368,18 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="45">
+    <row r="59" spans="1:17" ht="30">
       <c r="A59" s="46" t="s">
         <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E59" s="46" t="s">
-        <v>188</v>
+        <v>244</v>
       </c>
       <c r="K59" t="s">
         <v>114</v>
@@ -2398,7 +2399,7 @@
         <v>79</v>
       </c>
       <c r="E60" s="46" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="G60" t="s">
         <v>114</v>
@@ -2429,7 +2430,7 @@
         <v>102</v>
       </c>
       <c r="B62" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C62" s="16" t="s">
         <v>79</v>
@@ -2469,10 +2470,10 @@
     </row>
     <row r="64" spans="1:17">
       <c r="A64" s="46" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C64" s="47" t="s">
         <v>79</v>
@@ -2483,14 +2484,14 @@
     </row>
     <row r="65" spans="1:18" ht="30">
       <c r="A65" s="46" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B65" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C65" s="33"/>
       <c r="E65" s="46" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="Q65" t="s">
         <v>114</v>
@@ -2498,14 +2499,14 @@
     </row>
     <row r="66" spans="1:18">
       <c r="A66" s="46" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B66" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C66" s="33"/>
       <c r="E66" s="46" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="H66" t="s">
         <v>0</v>
@@ -2516,16 +2517,16 @@
     </row>
     <row r="67" spans="1:18" ht="30">
       <c r="A67" s="46" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B67" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C67" s="33" t="s">
         <v>79</v>
       </c>
       <c r="E67" s="46" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="H67" t="s">
         <v>23</v>
@@ -2533,16 +2534,16 @@
     </row>
     <row r="68" spans="1:18">
       <c r="A68" s="46" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="B68" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C68" s="58" t="s">
         <v>79</v>
       </c>
       <c r="E68" s="46" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="H68" t="s">
         <v>33</v>
@@ -2550,102 +2551,102 @@
     </row>
     <row r="69" spans="1:18">
       <c r="D69" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E69" s="46" t="s">
-        <v>198</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:18">
       <c r="D70" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E70" s="46" t="s">
-        <v>199</v>
+        <v>247</v>
       </c>
     </row>
     <row r="71" spans="1:18">
       <c r="B71" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C71" s="55"/>
       <c r="D71" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E71" s="46" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" ht="30">
       <c r="B72" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C72" s="55"/>
       <c r="D72" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E72" s="46" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
     </row>
     <row r="73" spans="1:18">
       <c r="B73" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C73" s="56"/>
       <c r="D73" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E73" s="46" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:18">
       <c r="B74" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C74" s="56"/>
       <c r="D74" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E74" s="46" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:18">
       <c r="B75" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C75" s="57"/>
       <c r="D75" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E75" s="46" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:18">
       <c r="B76" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C76" s="57"/>
       <c r="D76" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E76" s="46" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:18">
       <c r="B77" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C77" s="52"/>
       <c r="D77" t="s">
+        <v>162</v>
+      </c>
+      <c r="E77" s="46" t="s">
         <v>164</v>
-      </c>
-      <c r="E77" s="46" t="s">
-        <v>166</v>
       </c>
       <c r="R77" t="s">
         <v>114</v>
@@ -2653,14 +2654,14 @@
     </row>
     <row r="78" spans="1:18">
       <c r="B78" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C78" s="52"/>
       <c r="D78" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E78" s="46" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="R78" t="s">
         <v>114</v>
@@ -2668,14 +2669,14 @@
     </row>
     <row r="79" spans="1:18">
       <c r="B79" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C79" s="53"/>
       <c r="D79" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E79" s="46" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="R79" t="s">
         <v>114</v>
@@ -2683,14 +2684,14 @@
     </row>
     <row r="80" spans="1:18">
       <c r="B80" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C80" s="53"/>
       <c r="D80" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="E80" s="46" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="R80" t="s">
         <v>114</v>
@@ -2698,11 +2699,11 @@
     </row>
     <row r="81" spans="2:18">
       <c r="B81" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C81" s="54"/>
       <c r="E81" s="46" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R81" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Improved some comments in DCU code and DCU wiring spreadsheet. Rescaled overvoltage stress so balancing occurs at 3.51 V instead of 3.56 V. Rescaled undervoltage after first run-flat event, to give more warning. Zero at 3.1 V instead of 2.5 V. Added second set of stress offset and scale factors accessible by #define WHINGE 1. Allowed stress levels greater than 15 to be logged for querying by the 'q' command. Made Monitor send ID of temporary master every 17 seconds when there's a break in comms.
</commit_message>
<xml_diff>
--- a/master/tritium/DCU wiring.xlsx
+++ b/master/tritium/DCU wiring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="247">
   <si>
     <t>1A</t>
   </si>
@@ -324,9 +324,6 @@
     <t>Diag conn, Horn relay</t>
   </si>
   <si>
-    <t>Diag conn, Cooling fan relay</t>
-  </si>
-  <si>
     <t>Diag Conn, Tacho, Igniter</t>
   </si>
   <si>
@@ -459,9 +456,6 @@
     <t>WHT-GRN 2</t>
   </si>
   <si>
-    <t>BLK-GRN 2</t>
-  </si>
-  <si>
     <t>A2</t>
   </si>
   <si>
@@ -555,18 +549,6 @@
     <t>12V Always on (30A), Feeds Battery contactor relay contacts, From COOLING FAN fuse (repurposed)</t>
   </si>
   <si>
-    <t>B Battery contactors (12 V box DC-DC)</t>
-  </si>
-  <si>
-    <t>A Battery contactors (12 V box DC-DC)</t>
-  </si>
-  <si>
-    <t>B Battery contactors (B2 cont box)</t>
-  </si>
-  <si>
-    <t>A Battery contactors (A2 cont box)</t>
-  </si>
-  <si>
     <t>Fuel tank unit</t>
   </si>
   <si>
@@ -594,9 +576,6 @@
     <t>BRN 2</t>
   </si>
   <si>
-    <t>Crash switch NC, Joins WHT 3 at ECU/DCU location</t>
-  </si>
-  <si>
     <t>Crash switch</t>
   </si>
   <si>
@@ -624,9 +603,6 @@
     <t>Doesn't exist on our model</t>
   </si>
   <si>
-    <t>IGN_START</t>
-  </si>
-  <si>
     <t>Brakelight input</t>
   </si>
   <si>
@@ -702,29 +678,6 @@
     <t>Fuel tank unit, Fuel gauge (cut under dash)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Battery contactors (rear), connected to BRN or LGN-YEL under dash</t>
-    </r>
-  </si>
-  <si>
     <t>Fuel gauge, connected to BLU-ORG 2 under dash</t>
   </si>
   <si>
@@ -770,9 +723,6 @@
     <t>B9</t>
   </si>
   <si>
-    <t>A Battery contactors (rear), joined to BRN-YEL or WHT-GRN under dash</t>
-  </si>
-  <si>
     <t>Oil pressure gauge to oil pressure sensor, Joined to YEL-RED under dash</t>
   </si>
   <si>
@@ -780,13 +730,40 @@
   </si>
   <si>
     <t>Fuel door, Charge cable B detect</t>
+  </si>
+  <si>
+    <t>Joins BLK in A2 cont box to enable A/C</t>
+  </si>
+  <si>
+    <t>A Battery contactors (rear), disconnected from Circuit opening relay (fuel pump relay) under dash, joins BRN-YEL under dash</t>
+  </si>
+  <si>
+    <t>IGN_START, disconnect from Circuit opening relay (fuel pump relay) under dash</t>
+  </si>
+  <si>
+    <t>Crash switch NC, joins WHT 3 at ECU/DCU location</t>
+  </si>
+  <si>
+    <t>A Battery contactors (A2 cont box), joins BRN-YEL near DCUs</t>
+  </si>
+  <si>
+    <t>A Battery contactors (12 V box DC-DC), joins BLU-RED 2 under dash, joins BRN-YEL near DCUs</t>
+  </si>
+  <si>
+    <t>B Battery contactors (B2 cont box), joins BRN near DCUs</t>
+  </si>
+  <si>
+    <t>B Battery contactors (12 V box DC-DC), joins YEL 2 under dash, joins LGN-YEL near DCUs</t>
+  </si>
+  <si>
+    <t>B Battery contactors (rear), disconnected from fuel gauge under dash, joins BRN under dash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -797,14 +774,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1006,61 +975,61 @@
   </cellStyleXfs>
   <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1069,7 +1038,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1369,12 +1338,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R81"/>
+  <dimension ref="A1:R80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="750" activePane="bottomLeft"/>
+      <pane ySplit="750" topLeftCell="A52" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
+      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1389,63 +1358,63 @@
   <sheetData>
     <row r="1" spans="1:18" s="46" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B1" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="46" t="s">
-        <v>130</v>
-      </c>
       <c r="D1" s="46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G1" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="46" t="s">
         <v>115</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>116</v>
       </c>
       <c r="I1" s="46" t="s">
         <v>83</v>
       </c>
       <c r="J1" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="N1" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="O1" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="P1" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="K1" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="L1" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="M1" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="N1" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="O1" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="P1" s="46" t="s">
-        <v>136</v>
-      </c>
       <c r="Q1" s="46" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="R1" s="46" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
@@ -1454,10 +1423,10 @@
         <v>79</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1465,7 +1434,7 @@
     </row>
     <row r="3" spans="1:18" ht="30">
       <c r="A3" s="50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>45</v>
@@ -1474,24 +1443,24 @@
         <v>79</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="45">
       <c r="A4" s="46" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
@@ -1500,19 +1469,19 @@
         <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>202</v>
+        <v>240</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="30">
       <c r="A5" s="46" t="s">
         <v>81</v>
       </c>
@@ -1523,13 +1492,13 @@
         <v>79</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1543,7 +1512,7 @@
         <v>79</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -1563,19 +1532,19 @@
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="30">
       <c r="A8" s="46" t="s">
         <v>83</v>
       </c>
@@ -1586,16 +1555,16 @@
         <v>79</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>180</v>
+        <v>243</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="30">
       <c r="A9" s="46" t="s">
         <v>83</v>
       </c>
@@ -1606,13 +1575,13 @@
         <v>79</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>179</v>
+        <v>245</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1632,13 +1601,13 @@
         <v>79</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" ht="30">
       <c r="A12" s="46" t="s">
         <v>81</v>
       </c>
@@ -1649,13 +1618,13 @@
         <v>79</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>181</v>
+        <v>244</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1681,16 +1650,16 @@
         <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
       </c>
       <c r="O15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1704,10 +1673,10 @@
         <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -1724,10 +1693,10 @@
         <v>79</v>
       </c>
       <c r="D17" t="s">
+        <v>196</v>
+      </c>
+      <c r="E17" s="46" t="s">
         <v>204</v>
-      </c>
-      <c r="E17" s="46" t="s">
-        <v>212</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -1744,7 +1713,7 @@
         <v>79</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -1760,13 +1729,19 @@
       <c r="C19" s="16" t="s">
         <v>79</v>
       </c>
+      <c r="E19" s="46" t="s">
+        <v>238</v>
+      </c>
       <c r="F19" t="s">
         <v>17</v>
       </c>
+      <c r="G19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="20" spans="1:16" ht="30">
       <c r="A20" s="46" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
@@ -1775,7 +1750,7 @@
         <v>79</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
@@ -1812,16 +1787,16 @@
         <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F23" t="s">
         <v>21</v>
       </c>
       <c r="P23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1854,7 +1829,7 @@
     </row>
     <row r="26" spans="1:16" ht="30">
       <c r="A26" s="46" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B26" t="s">
         <v>65</v>
@@ -1863,24 +1838,24 @@
         <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F26" t="s">
         <v>24</v>
       </c>
       <c r="M26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="30">
       <c r="A27" s="46" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
@@ -1889,19 +1864,19 @@
         <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F27" t="s">
         <v>25</v>
       </c>
       <c r="M27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -1915,16 +1890,16 @@
         <v>79</v>
       </c>
       <c r="D28" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" s="46" t="s">
         <v>168</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>170</v>
       </c>
       <c r="F28" t="s">
         <v>26</v>
       </c>
       <c r="N28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1944,21 +1919,21 @@
         <v>79</v>
       </c>
       <c r="D30" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30" s="46" t="s">
         <v>169</v>
-      </c>
-      <c r="E30" s="46" t="s">
-        <v>171</v>
       </c>
       <c r="F30" t="s">
         <v>28</v>
       </c>
       <c r="N30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
         <v>70</v>
@@ -1967,7 +1942,7 @@
         <v>79</v>
       </c>
       <c r="E31" s="46" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F31" t="s">
         <v>29</v>
@@ -1984,16 +1959,16 @@
         <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F32" t="s">
         <v>30</v>
       </c>
       <c r="I32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -2004,7 +1979,7 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
         <v>72</v>
@@ -2016,7 +1991,7 @@
         <v>32</v>
       </c>
       <c r="M34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -2030,21 +2005,21 @@
         <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F35" t="s">
         <v>33</v>
       </c>
       <c r="O35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B36" t="s">
         <v>57</v>
@@ -2058,10 +2033,10 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C37" s="29" t="s">
         <v>79</v>
@@ -2072,10 +2047,10 @@
     </row>
     <row r="38" spans="1:15" ht="30">
       <c r="A38" s="46" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B38" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>79</v>
@@ -2084,12 +2059,12 @@
         <v>36</v>
       </c>
       <c r="M38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
         <v>74</v>
@@ -2101,12 +2076,12 @@
         <v>37</v>
       </c>
       <c r="M39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" t="s">
         <v>75</v>
@@ -2115,7 +2090,7 @@
         <v>79</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="F40" t="s">
         <v>38</v>
@@ -2141,7 +2116,7 @@
     </row>
     <row r="44" spans="1:15" ht="30">
       <c r="A44" s="46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
         <v>76</v>
@@ -2150,7 +2125,7 @@
         <v>79</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F44" t="s">
         <v>42</v>
@@ -2158,16 +2133,19 @@
     </row>
     <row r="45" spans="1:15" ht="30">
       <c r="A45" s="46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>79</v>
       </c>
+      <c r="D45" t="s">
+        <v>163</v>
+      </c>
       <c r="E45" s="46" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F45" t="s">
         <v>43</v>
@@ -2175,19 +2153,19 @@
     </row>
     <row r="46" spans="1:15" ht="30">
       <c r="A46" s="46" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B46" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F46" t="s">
         <v>60</v>
@@ -2195,16 +2173,16 @@
     </row>
     <row r="47" spans="1:15" ht="30">
       <c r="A47" s="46" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B47" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>79</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F47" t="s">
         <v>60</v>
@@ -2212,7 +2190,7 @@
     </row>
     <row r="48" spans="1:15" ht="30">
       <c r="A48" s="46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B48" t="s">
         <v>77</v>
@@ -2221,10 +2199,10 @@
         <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F48" t="s">
         <v>61</v>
@@ -2251,16 +2229,16 @@
     </row>
     <row r="52" spans="1:17" ht="45">
       <c r="A52" s="46" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B52" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>79</v>
       </c>
       <c r="E52" s="46" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -2268,13 +2246,13 @@
         <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C53" s="41" t="s">
         <v>79</v>
       </c>
       <c r="L53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:17">
@@ -2282,47 +2260,47 @@
         <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C54" s="25" t="s">
         <v>79</v>
       </c>
       <c r="L54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:17">
       <c r="A55" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>79</v>
       </c>
       <c r="I55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:17">
       <c r="A56" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C56" s="42" t="s">
         <v>79</v>
       </c>
       <c r="I56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -2336,61 +2314,61 @@
         <v>79</v>
       </c>
       <c r="I57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:17">
       <c r="A58" s="46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>79</v>
       </c>
       <c r="E58" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H58" t="s">
         <v>7</v>
       </c>
       <c r="I58" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" ht="30">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="45">
       <c r="A59" s="46" t="s">
         <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E59" s="46" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="K59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="30">
       <c r="A60" s="46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B60" t="s">
         <v>78</v>
@@ -2399,16 +2377,16 @@
         <v>79</v>
       </c>
       <c r="E60" s="46" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="G60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -2422,291 +2400,277 @@
         <v>79</v>
       </c>
       <c r="G61" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="30">
       <c r="A62" s="46" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>147</v>
-      </c>
-      <c r="C62" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" s="45" t="s">
         <v>79</v>
       </c>
       <c r="G62" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" ht="30">
+        <v>113</v>
+      </c>
+      <c r="I62" t="s">
+        <v>122</v>
+      </c>
+      <c r="K62" t="s">
+        <v>113</v>
+      </c>
+      <c r="L62" t="s">
+        <v>113</v>
+      </c>
+      <c r="M62" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
       <c r="A63" s="46" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
-      </c>
-      <c r="C63" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="G63" t="s">
-        <v>114</v>
-      </c>
-      <c r="I63" t="s">
-        <v>123</v>
-      </c>
-      <c r="K63" t="s">
-        <v>114</v>
-      </c>
-      <c r="L63" t="s">
-        <v>114</v>
-      </c>
-      <c r="M63" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17">
+        <v>136</v>
+      </c>
+      <c r="C63" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="P63" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="30">
       <c r="A64" s="46" t="s">
-        <v>136</v>
+        <v>219</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="P64" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" ht="30">
+        <v>178</v>
+      </c>
+      <c r="C64" s="33"/>
+      <c r="E64" s="46" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
       <c r="A65" s="46" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B65" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="C65" s="33"/>
       <c r="E65" s="46" t="s">
-        <v>228</v>
+        <v>220</v>
+      </c>
+      <c r="H65" t="s">
+        <v>0</v>
       </c>
       <c r="Q65" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" ht="30">
       <c r="A66" s="46" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="B66" t="s">
+        <v>192</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E66" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="H66" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
+      <c r="A67" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="B67" t="s">
+        <v>222</v>
+      </c>
+      <c r="C67" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="E67" s="46" t="s">
         <v>224</v>
       </c>
-      <c r="C66" s="33"/>
-      <c r="E66" s="46" t="s">
-        <v>229</v>
-      </c>
-      <c r="H66" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" ht="30">
-      <c r="A67" s="46" t="s">
-        <v>219</v>
-      </c>
-      <c r="B67" t="s">
-        <v>199</v>
-      </c>
-      <c r="C67" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="E67" s="46" t="s">
-        <v>245</v>
-      </c>
       <c r="H67" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:18">
-      <c r="A68" s="46" t="s">
-        <v>230</v>
-      </c>
-      <c r="B68" t="s">
-        <v>231</v>
-      </c>
-      <c r="C68" s="58" t="s">
-        <v>79</v>
+      <c r="D68" t="s">
+        <v>150</v>
       </c>
       <c r="E68" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="H68" t="s">
-        <v>33</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="1:18">
       <c r="D69" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E69" s="46" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="70" spans="1:18">
+      <c r="B70" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70" s="55"/>
       <c r="D70" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E70" s="46" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" ht="30">
       <c r="B71" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C71" s="55"/>
       <c r="D71" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E71" s="46" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" ht="30">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
       <c r="B72" t="s">
-        <v>195</v>
-      </c>
-      <c r="C72" s="55"/>
+        <v>189</v>
+      </c>
+      <c r="C72" s="56"/>
       <c r="D72" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="E72" s="46" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="73" spans="1:18">
       <c r="B73" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C73" s="56"/>
       <c r="D73" t="s">
-        <v>216</v>
+        <v>157</v>
       </c>
       <c r="E73" s="46" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="74" spans="1:18">
       <c r="B74" t="s">
-        <v>196</v>
-      </c>
-      <c r="C74" s="56"/>
+        <v>190</v>
+      </c>
+      <c r="C74" s="57"/>
       <c r="D74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E74" s="46" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75" spans="1:18">
       <c r="B75" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C75" s="57"/>
       <c r="D75" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E75" s="46" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="76" spans="1:18">
       <c r="B76" t="s">
-        <v>197</v>
-      </c>
-      <c r="C76" s="57"/>
+        <v>185</v>
+      </c>
+      <c r="C76" s="52"/>
       <c r="D76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E76" s="46" t="s">
-        <v>240</v>
+        <v>162</v>
+      </c>
+      <c r="R76" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:18">
       <c r="B77" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C77" s="52"/>
       <c r="D77" t="s">
+        <v>161</v>
+      </c>
+      <c r="E77" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="E77" s="46" t="s">
-        <v>164</v>
-      </c>
       <c r="R77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:18">
       <c r="B78" t="s">
-        <v>191</v>
-      </c>
-      <c r="C78" s="52"/>
+        <v>183</v>
+      </c>
+      <c r="C78" s="53"/>
       <c r="D78" t="s">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="E78" s="46" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
       <c r="R78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:18">
       <c r="B79" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C79" s="53"/>
       <c r="D79" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="E79" s="46" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="R79" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="80" spans="1:18">
       <c r="B80" t="s">
-        <v>189</v>
-      </c>
-      <c r="C80" s="53"/>
-      <c r="D80" t="s">
-        <v>243</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C80" s="54"/>
       <c r="E80" s="46" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="R80" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="81" spans="2:18">
-      <c r="B81" t="s">
-        <v>190</v>
-      </c>
-      <c r="C81" s="54"/>
-      <c r="E81" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="R81" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Apply a slew-rate-limit to torque zero-crossings in process_pedal() to try to avoid problems with backlash causing clutch slip.
In DCU wiring.xlsx, remove the BLK-LGN from DCU-B (pin B2).
</commit_message>
<xml_diff>
--- a/master/tritium/DCU wiring.xlsx
+++ b/master/tritium/DCU wiring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="246">
   <si>
     <t>1A</t>
   </si>
@@ -457,9 +457,6 @@
   </si>
   <si>
     <t>A2</t>
-  </si>
-  <si>
-    <t>B2</t>
   </si>
   <si>
     <t>A20</t>
@@ -1341,9 +1338,9 @@
   <dimension ref="A1:R80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="750" topLeftCell="A52" activePane="bottomLeft"/>
+      <pane ySplit="750" topLeftCell="A9" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1358,7 +1355,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="46" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>128</v>
@@ -1370,10 +1367,10 @@
         <v>133</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G1" s="46" t="s">
         <v>114</v>
@@ -1406,10 +1403,10 @@
         <v>135</v>
       </c>
       <c r="Q1" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R1" s="46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1423,10 +1420,10 @@
         <v>79</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1443,7 +1440,7 @@
         <v>79</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -1460,7 +1457,7 @@
     </row>
     <row r="4" spans="1:18" ht="45">
       <c r="A4" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
@@ -1469,10 +1466,10 @@
         <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
@@ -1492,7 +1489,7 @@
         <v>79</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -1512,7 +1509,7 @@
         <v>79</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -1532,10 +1529,10 @@
         <v>79</v>
       </c>
       <c r="D7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" s="46" t="s">
         <v>163</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>164</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
@@ -1555,7 +1552,7 @@
         <v>79</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -1575,7 +1572,7 @@
         <v>79</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -1601,7 +1598,7 @@
         <v>79</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -1618,7 +1615,7 @@
         <v>79</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -1650,10 +1647,10 @@
         <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
@@ -1673,10 +1670,10 @@
         <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -1693,10 +1690,10 @@
         <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -1713,7 +1710,7 @@
         <v>79</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -1730,7 +1727,7 @@
         <v>79</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -1741,7 +1738,7 @@
     </row>
     <row r="20" spans="1:16" ht="30">
       <c r="A20" s="46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
@@ -1750,7 +1747,7 @@
         <v>79</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
@@ -1790,7 +1787,7 @@
         <v>137</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F23" t="s">
         <v>21</v>
@@ -1829,7 +1826,7 @@
     </row>
     <row r="26" spans="1:16" ht="30">
       <c r="A26" s="46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B26" t="s">
         <v>65</v>
@@ -1855,16 +1852,13 @@
     </row>
     <row r="27" spans="1:16" ht="30">
       <c r="A27" s="46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>79</v>
-      </c>
-      <c r="D27" t="s">
-        <v>147</v>
       </c>
       <c r="F27" t="s">
         <v>25</v>
@@ -1890,10 +1884,10 @@
         <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E28" s="46" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F28" t="s">
         <v>26</v>
@@ -1919,10 +1913,10 @@
         <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E30" s="46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F30" t="s">
         <v>28</v>
@@ -1942,7 +1936,7 @@
         <v>79</v>
       </c>
       <c r="E31" s="46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F31" t="s">
         <v>29</v>
@@ -1962,7 +1956,7 @@
         <v>139</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F32" t="s">
         <v>30</v>
@@ -2005,10 +1999,10 @@
         <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F35" t="s">
         <v>33</v>
@@ -2036,7 +2030,7 @@
         <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C37" s="29" t="s">
         <v>79</v>
@@ -2047,10 +2041,10 @@
     </row>
     <row r="38" spans="1:15" ht="30">
       <c r="A38" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>79</v>
@@ -2090,7 +2084,7 @@
         <v>79</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F40" t="s">
         <v>38</v>
@@ -2125,7 +2119,7 @@
         <v>79</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F44" t="s">
         <v>42</v>
@@ -2136,16 +2130,16 @@
         <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F45" t="s">
         <v>43</v>
@@ -2153,19 +2147,19 @@
     </row>
     <row r="46" spans="1:15" ht="30">
       <c r="A46" s="46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F46" t="s">
         <v>60</v>
@@ -2173,16 +2167,16 @@
     </row>
     <row r="47" spans="1:15" ht="30">
       <c r="A47" s="46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>79</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F47" t="s">
         <v>60</v>
@@ -2199,10 +2193,10 @@
         <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F48" t="s">
         <v>61</v>
@@ -2229,16 +2223,16 @@
     </row>
     <row r="52" spans="1:17" ht="45">
       <c r="A52" s="46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B52" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>79</v>
       </c>
       <c r="E52" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -2357,7 +2351,7 @@
         <v>79</v>
       </c>
       <c r="E59" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K59" t="s">
         <v>113</v>
@@ -2377,7 +2371,7 @@
         <v>79</v>
       </c>
       <c r="E60" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G60" t="s">
         <v>113</v>
@@ -2448,14 +2442,14 @@
     </row>
     <row r="64" spans="1:17" ht="30">
       <c r="A64" s="46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B64" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C64" s="33"/>
       <c r="E64" s="46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q64" t="s">
         <v>113</v>
@@ -2463,14 +2457,14 @@
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B65" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C65" s="33"/>
       <c r="E65" s="46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H65" t="s">
         <v>0</v>
@@ -2481,16 +2475,16 @@
     </row>
     <row r="66" spans="1:18" ht="30">
       <c r="A66" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B66" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C66" s="33" t="s">
         <v>79</v>
       </c>
       <c r="E66" s="46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H66" t="s">
         <v>23</v>
@@ -2498,16 +2492,16 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="B67" t="s">
         <v>221</v>
       </c>
-      <c r="B67" t="s">
-        <v>222</v>
-      </c>
       <c r="C67" s="58" t="s">
         <v>79</v>
       </c>
       <c r="E67" s="46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H67" t="s">
         <v>33</v>
@@ -2515,102 +2509,102 @@
     </row>
     <row r="68" spans="1:18">
       <c r="D68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E68" s="46" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:18">
       <c r="D69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E69" s="46" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="70" spans="1:18">
       <c r="B70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C70" s="55"/>
       <c r="D70" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E70" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="30">
       <c r="B71" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C71" s="55"/>
       <c r="D71" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E71" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="72" spans="1:18">
       <c r="B72" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C72" s="56"/>
       <c r="D72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E72" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73" spans="1:18">
       <c r="B73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C73" s="56"/>
       <c r="D73" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E73" s="46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="74" spans="1:18">
       <c r="B74" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C74" s="57"/>
       <c r="D74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E74" s="46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="75" spans="1:18">
       <c r="B75" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C75" s="57"/>
       <c r="D75" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E75" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:18">
       <c r="B76" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C76" s="52"/>
       <c r="D76" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E76" s="46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R76" t="s">
         <v>113</v>
@@ -2618,14 +2612,14 @@
     </row>
     <row r="77" spans="1:18">
       <c r="B77" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C77" s="52"/>
       <c r="D77" t="s">
+        <v>160</v>
+      </c>
+      <c r="E77" s="46" t="s">
         <v>161</v>
-      </c>
-      <c r="E77" s="46" t="s">
-        <v>162</v>
       </c>
       <c r="R77" t="s">
         <v>113</v>
@@ -2633,14 +2627,14 @@
     </row>
     <row r="78" spans="1:18">
       <c r="B78" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C78" s="53"/>
       <c r="D78" t="s">
+        <v>208</v>
+      </c>
+      <c r="E78" s="46" t="s">
         <v>209</v>
-      </c>
-      <c r="E78" s="46" t="s">
-        <v>210</v>
       </c>
       <c r="R78" t="s">
         <v>113</v>
@@ -2648,14 +2642,14 @@
     </row>
     <row r="79" spans="1:18">
       <c r="B79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C79" s="53"/>
       <c r="D79" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E79" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="R79" t="s">
         <v>113</v>
@@ -2663,11 +2657,11 @@
     </row>
     <row r="80" spans="1:18">
       <c r="B80" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C80" s="54"/>
       <c r="E80" s="46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R80" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Moved 100 Hz tick timing from Timer A to Timer B, to free up Timer A for a possible software UART. Updated DCU wiring spreadsheet and diagram. Added DCU mods for stronger pullups and pulldowns.
</commit_message>
<xml_diff>
--- a/master/tritium/DCU wiring.xlsx
+++ b/master/tritium/DCU wiring.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterate="1" iterateCount="1" iterateDelta="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="247">
   <si>
     <t>1A</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t>B Battery contactors (rear), disconnected from fuel gauge under dash, joins BRN under dash</t>
+  </si>
+  <si>
+    <t>A18</t>
   </si>
 </sst>
 </file>
@@ -1338,9 +1341,9 @@
   <dimension ref="A1:R80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="750" topLeftCell="A9" activePane="bottomLeft"/>
+      <pane ySplit="750" topLeftCell="A55" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2082,6 +2085,9 @@
       </c>
       <c r="C40" s="31" t="s">
         <v>79</v>
+      </c>
+      <c r="D40" t="s">
+        <v>246</v>
       </c>
       <c r="E40" s="46" t="s">
         <v>222</v>

</xml_diff>

<commit_message>
Updated the DCU wring diagram and spreadsheet to show the new and revised pin assignments due to adding the 3rd UART (this one in software) for the voice synthesizer. Updated the DCU modification instructions to include the mods to bring out the 3rd UART on the DC37 connector (pins 28 and 10, were GEAR 3 and 4). Updated the DCU modification instructions to eliminate the obsolete instructions for bring out the two hardware UARTs on the DC37 and instead included instructions for bringing them out on the IFO connectors as we have been doing for quite some time.
</commit_message>
<xml_diff>
--- a/master/tritium/DCU wiring.xlsx
+++ b/master/tritium/DCU wiring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="251">
   <si>
     <t>1A</t>
   </si>
@@ -525,9 +525,6 @@
     <t>B Charging contactor</t>
   </si>
   <si>
-    <t>Gear4, Neutral or Clutch</t>
-  </si>
-  <si>
     <t>+5V to Accelerator potbox</t>
   </si>
   <si>
@@ -699,12 +696,6 @@
     <t>LED Gear 4, Non-pedal DCU presence out, joined to A24</t>
   </si>
   <si>
-    <t>Gear 3 input, Inhibit traction in, joined to B13</t>
-  </si>
-  <si>
-    <t>LED Gear 3, DCU-B in charge mode out, joined to A7</t>
-  </si>
-  <si>
     <t>Brakelight input, request brakelight in, joined to A13</t>
   </si>
   <si>
@@ -757,6 +748,27 @@
   </si>
   <si>
     <t>A18</t>
+  </si>
+  <si>
+    <t>A29</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>Gear4, Neutral or Clutch (was A10)</t>
+  </si>
+  <si>
+    <t>Gear 3 input, Inhibit traction in, joined to B13 (was A28)</t>
+  </si>
+  <si>
+    <t>LED Gear 3, DCU-B-in-charge-mode out, joined to A29 (was joined to A28)</t>
+  </si>
+  <si>
+    <t>Voice synth RX (Gear 3)</t>
+  </si>
+  <si>
+    <t>Voice Synth TX (Gear 4)</t>
   </si>
 </sst>
 </file>
@@ -1338,12 +1350,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R80"/>
+  <dimension ref="A1:R82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="750" topLeftCell="A55" activePane="bottomLeft"/>
+      <pane ySplit="750" topLeftCell="A60" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomLeft" activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1358,7 +1370,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="46" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>128</v>
@@ -1370,10 +1382,10 @@
         <v>133</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G1" s="46" t="s">
         <v>114</v>
@@ -1406,10 +1418,10 @@
         <v>135</v>
       </c>
       <c r="Q1" s="46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R1" s="46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1426,7 +1438,7 @@
         <v>164</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1443,7 +1455,7 @@
         <v>79</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -1460,7 +1472,7 @@
     </row>
     <row r="4" spans="1:18" ht="45">
       <c r="A4" s="46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
@@ -1472,7 +1484,7 @@
         <v>151</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
@@ -1492,7 +1504,7 @@
         <v>79</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -1512,7 +1524,7 @@
         <v>79</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -1555,7 +1567,7 @@
         <v>79</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -1575,7 +1587,7 @@
         <v>79</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -1601,7 +1613,7 @@
         <v>79</v>
       </c>
       <c r="E11" s="46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -1618,7 +1630,7 @@
         <v>79</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -1653,7 +1665,7 @@
         <v>148</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
@@ -1676,7 +1688,7 @@
         <v>155</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -1693,10 +1705,10 @@
         <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -1713,7 +1725,7 @@
         <v>79</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
@@ -1730,7 +1742,7 @@
         <v>79</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -1741,7 +1753,7 @@
     </row>
     <row r="20" spans="1:16" ht="30">
       <c r="A20" s="46" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
@@ -1750,7 +1762,7 @@
         <v>79</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
@@ -1787,10 +1799,10 @@
         <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>245</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>169</v>
+        <v>246</v>
       </c>
       <c r="F23" t="s">
         <v>21</v>
@@ -1829,7 +1841,7 @@
     </row>
     <row r="26" spans="1:16" ht="30">
       <c r="A26" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B26" t="s">
         <v>65</v>
@@ -1855,7 +1867,7 @@
     </row>
     <row r="27" spans="1:16" ht="30">
       <c r="A27" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
@@ -1939,7 +1951,7 @@
         <v>79</v>
       </c>
       <c r="E31" s="46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F31" t="s">
         <v>29</v>
@@ -1959,7 +1971,7 @@
         <v>139</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F32" t="s">
         <v>30</v>
@@ -2005,7 +2017,7 @@
         <v>147</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F35" t="s">
         <v>33</v>
@@ -2033,7 +2045,7 @@
         <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C37" s="29" t="s">
         <v>79</v>
@@ -2044,10 +2056,10 @@
     </row>
     <row r="38" spans="1:15" ht="30">
       <c r="A38" s="46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>79</v>
@@ -2087,10 +2099,10 @@
         <v>79</v>
       </c>
       <c r="D40" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F40" t="s">
         <v>38</v>
@@ -2125,7 +2137,7 @@
         <v>79</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F44" t="s">
         <v>42</v>
@@ -2145,7 +2157,7 @@
         <v>162</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F45" t="s">
         <v>43</v>
@@ -2153,19 +2165,19 @@
     </row>
     <row r="46" spans="1:15" ht="30">
       <c r="A46" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F46" t="s">
         <v>60</v>
@@ -2173,16 +2185,16 @@
     </row>
     <row r="47" spans="1:15" ht="30">
       <c r="A47" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>79</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F47" t="s">
         <v>60</v>
@@ -2199,10 +2211,10 @@
         <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F48" t="s">
         <v>61</v>
@@ -2229,16 +2241,16 @@
     </row>
     <row r="52" spans="1:17" ht="45">
       <c r="A52" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B52" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>79</v>
       </c>
       <c r="E52" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -2357,7 +2369,7 @@
         <v>79</v>
       </c>
       <c r="E59" s="46" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K59" t="s">
         <v>113</v>
@@ -2377,7 +2389,7 @@
         <v>79</v>
       </c>
       <c r="E60" s="46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G60" t="s">
         <v>113</v>
@@ -2448,14 +2460,14 @@
     </row>
     <row r="64" spans="1:17" ht="30">
       <c r="A64" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C64" s="33"/>
       <c r="E64" s="46" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="Q64" t="s">
         <v>113</v>
@@ -2463,14 +2475,14 @@
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B65" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C65" s="33"/>
       <c r="E65" s="46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H65" t="s">
         <v>0</v>
@@ -2481,16 +2493,16 @@
     </row>
     <row r="66" spans="1:18" ht="30">
       <c r="A66" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C66" s="33" t="s">
         <v>79</v>
       </c>
       <c r="E66" s="46" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H66" t="s">
         <v>23</v>
@@ -2498,16 +2510,16 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="B67" t="s">
         <v>220</v>
       </c>
-      <c r="B67" t="s">
-        <v>221</v>
-      </c>
       <c r="C67" s="58" t="s">
         <v>79</v>
       </c>
       <c r="E67" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H67" t="s">
         <v>33</v>
@@ -2518,7 +2530,7 @@
         <v>149</v>
       </c>
       <c r="E68" s="46" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:18">
@@ -2526,84 +2538,84 @@
         <v>150</v>
       </c>
       <c r="E69" s="46" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70" spans="1:18">
       <c r="B70" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C70" s="55"/>
       <c r="D70" t="s">
         <v>153</v>
       </c>
       <c r="E70" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="30">
       <c r="B71" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C71" s="55"/>
       <c r="D71" t="s">
         <v>154</v>
       </c>
       <c r="E71" s="46" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" ht="30">
       <c r="B72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C72" s="56"/>
       <c r="D72" t="s">
-        <v>207</v>
+        <v>244</v>
       </c>
       <c r="E72" s="46" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" ht="30">
       <c r="B73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C73" s="56"/>
       <c r="D73" t="s">
         <v>156</v>
       </c>
       <c r="E73" s="46" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
     </row>
     <row r="74" spans="1:18">
       <c r="B74" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C74" s="57"/>
       <c r="D74" t="s">
         <v>157</v>
       </c>
       <c r="E74" s="46" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="75" spans="1:18">
       <c r="B75" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C75" s="57"/>
       <c r="D75" t="s">
         <v>158</v>
       </c>
       <c r="E75" s="46" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="76" spans="1:18">
       <c r="B76" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C76" s="52"/>
       <c r="D76" t="s">
@@ -2618,7 +2630,7 @@
     </row>
     <row r="77" spans="1:18">
       <c r="B77" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C77" s="52"/>
       <c r="D77" t="s">
@@ -2633,14 +2645,14 @@
     </row>
     <row r="78" spans="1:18">
       <c r="B78" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C78" s="53"/>
       <c r="D78" t="s">
+        <v>207</v>
+      </c>
+      <c r="E78" s="46" t="s">
         <v>208</v>
-      </c>
-      <c r="E78" s="46" t="s">
-        <v>209</v>
       </c>
       <c r="R78" t="s">
         <v>113</v>
@@ -2648,14 +2660,14 @@
     </row>
     <row r="79" spans="1:18">
       <c r="B79" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C79" s="53"/>
       <c r="D79" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E79" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="R79" t="s">
         <v>113</v>
@@ -2663,14 +2675,30 @@
     </row>
     <row r="80" spans="1:18">
       <c r="B80" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C80" s="54"/>
       <c r="E80" s="46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R80" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="4:5">
+      <c r="D81" t="s">
+        <v>206</v>
+      </c>
+      <c r="E81" s="46" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="82" spans="4:5">
+      <c r="D82" t="s">
+        <v>137</v>
+      </c>
+      <c r="E82" s="46" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code and updated wiring spreadsheet and diagram to use the LED_FAULT_2 output (DC37 pin 34) to drive a loud piezo beeper as a cell stress alarm when stress goes to 11 or more.
</commit_message>
<xml_diff>
--- a/master/tritium/DCU wiring.xlsx
+++ b/master/tritium/DCU wiring.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" iterate="1" iterateCount="1" iterateDelta="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="253">
   <si>
     <t>1A</t>
   </si>
@@ -769,6 +770,12 @@
   </si>
   <si>
     <t>Voice Synth TX (Gear 4)</t>
+  </si>
+  <si>
+    <t>LED_FAULT_2, loud piezo beeper under dash on driver's side (cell stress &gt;= 11 alarm)</t>
+  </si>
+  <si>
+    <t>A34</t>
   </si>
 </sst>
 </file>
@@ -1350,12 +1357,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R82"/>
+  <dimension ref="A1:R83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="750" topLeftCell="A60" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E82" sqref="E82"/>
+      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2699,6 +2706,14 @@
       </c>
       <c r="E82" s="46" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="83" spans="4:5" ht="30">
+      <c r="D83" t="s">
+        <v>252</v>
+      </c>
+      <c r="E83" s="46" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated wiring spreadsheet to include: LGN: Joined to RED-BLU under the dash, Powers IMUs in contactor boxes A2 and B2.
</commit_message>
<xml_diff>
--- a/master/tritium/DCU wiring.xlsx
+++ b/master/tritium/DCU wiring.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" iterate="1" iterateCount="1" iterateDelta="0"/>
+  <calcPr calcId="125725"/>
   <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
@@ -538,9 +538,6 @@
     <t>Joins LGN-BLK to enable A/C</t>
   </si>
   <si>
-    <t>+12V Always on (10A)</t>
-  </si>
-  <si>
     <t>12V Always on (30A), Feeds Battery contactor relay contacts, From COOLING FAN fuse (repurposed)</t>
   </si>
   <si>
@@ -658,15 +655,9 @@
     <t>Airflow meter (not in 12V box, prob near diag conn)</t>
   </si>
   <si>
-    <t>Carries TRACTION signal to Pumps relay in 12V box, Joins LGN under dash</t>
-  </si>
-  <si>
     <t>YEL 3</t>
   </si>
   <si>
-    <t>Joins YEL-BLK 2 under dash</t>
-  </si>
-  <si>
     <t>Connected to Fuel gauge YEL 3 under dash, Gauge4</t>
   </si>
   <si>
@@ -776,6 +767,15 @@
   </si>
   <si>
     <t>A34</t>
+  </si>
+  <si>
+    <t>+12V Always on (10A), connected to LGN under dash</t>
+  </si>
+  <si>
+    <t>Carries TRACTION signal to Pumps relay in 12V box</t>
+  </si>
+  <si>
+    <t>Joined to RED-BLU under the dash, Powers IMUs in contactor boxes A2 and B2</t>
   </si>
 </sst>
 </file>
@@ -1360,9 +1360,9 @@
   <dimension ref="A1:R83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="750" topLeftCell="A60" activePane="bottomLeft"/>
+      <pane ySplit="750" topLeftCell="A48" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
+      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1377,7 +1377,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="46" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>128</v>
@@ -1389,10 +1389,10 @@
         <v>133</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G1" s="46" t="s">
         <v>114</v>
@@ -1425,10 +1425,10 @@
         <v>135</v>
       </c>
       <c r="Q1" s="46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R1" s="46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1445,7 +1445,7 @@
         <v>164</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>173</v>
+        <v>250</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         <v>79</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -1479,7 +1479,7 @@
     </row>
     <row r="4" spans="1:18" ht="45">
       <c r="A4" s="46" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
@@ -1491,7 +1491,7 @@
         <v>151</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
@@ -1511,7 +1511,7 @@
         <v>79</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -1531,7 +1531,7 @@
         <v>79</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -1574,7 +1574,7 @@
         <v>79</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -1594,7 +1594,7 @@
         <v>79</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -1637,7 +1637,7 @@
         <v>79</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -1695,7 +1695,7 @@
         <v>155</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -1712,10 +1712,10 @@
         <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -1749,7 +1749,7 @@
         <v>79</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="20" spans="1:16" ht="30">
       <c r="A20" s="46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
@@ -1769,7 +1769,7 @@
         <v>79</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
@@ -1806,10 +1806,10 @@
         <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F23" t="s">
         <v>21</v>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="26" spans="1:16" ht="30">
       <c r="A26" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B26" t="s">
         <v>65</v>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="27" spans="1:16" ht="30">
       <c r="A27" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
@@ -1958,7 +1958,7 @@
         <v>79</v>
       </c>
       <c r="E31" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F31" t="s">
         <v>29</v>
@@ -1978,7 +1978,7 @@
         <v>139</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F32" t="s">
         <v>30</v>
@@ -2052,7 +2052,7 @@
         <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C37" s="29" t="s">
         <v>79</v>
@@ -2063,10 +2063,10 @@
     </row>
     <row r="38" spans="1:15" ht="30">
       <c r="A38" s="46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>79</v>
@@ -2106,10 +2106,10 @@
         <v>79</v>
       </c>
       <c r="D40" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F40" t="s">
         <v>38</v>
@@ -2144,13 +2144,13 @@
         <v>79</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="30">
+    <row r="45" spans="1:15">
       <c r="A45" s="46" t="s">
         <v>111</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>162</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="F45" t="s">
         <v>43</v>
@@ -2172,19 +2172,19 @@
     </row>
     <row r="46" spans="1:15" ht="30">
       <c r="A46" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F46" t="s">
         <v>60</v>
@@ -2192,16 +2192,16 @@
     </row>
     <row r="47" spans="1:15" ht="30">
       <c r="A47" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>79</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F47" t="s">
         <v>60</v>
@@ -2218,10 +2218,10 @@
         <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F48" t="s">
         <v>61</v>
@@ -2248,16 +2248,16 @@
     </row>
     <row r="52" spans="1:17" ht="45">
       <c r="A52" s="46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>79</v>
       </c>
       <c r="E52" s="46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -2376,7 +2376,7 @@
         <v>79</v>
       </c>
       <c r="E59" s="46" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="K59" t="s">
         <v>113</v>
@@ -2396,7 +2396,7 @@
         <v>79</v>
       </c>
       <c r="E60" s="46" t="s">
-        <v>215</v>
+        <v>252</v>
       </c>
       <c r="G60" t="s">
         <v>113</v>
@@ -2467,14 +2467,14 @@
     </row>
     <row r="64" spans="1:17" ht="30">
       <c r="A64" s="46" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C64" s="33"/>
       <c r="E64" s="46" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="Q64" t="s">
         <v>113</v>
@@ -2482,14 +2482,14 @@
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="46" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B65" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C65" s="33"/>
       <c r="E65" s="46" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H65" t="s">
         <v>0</v>
@@ -2500,16 +2500,16 @@
     </row>
     <row r="66" spans="1:18" ht="30">
       <c r="A66" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66" s="33" t="s">
         <v>79</v>
       </c>
       <c r="E66" s="46" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H66" t="s">
         <v>23</v>
@@ -2517,16 +2517,16 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="B67" t="s">
+        <v>217</v>
+      </c>
+      <c r="C67" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="E67" s="46" t="s">
         <v>219</v>
-      </c>
-      <c r="B67" t="s">
-        <v>220</v>
-      </c>
-      <c r="C67" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="E67" s="46" t="s">
-        <v>222</v>
       </c>
       <c r="H67" t="s">
         <v>33</v>
@@ -2537,7 +2537,7 @@
         <v>149</v>
       </c>
       <c r="E68" s="46" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" spans="1:18">
@@ -2545,84 +2545,84 @@
         <v>150</v>
       </c>
       <c r="E69" s="46" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="70" spans="1:18">
       <c r="B70" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C70" s="55"/>
       <c r="D70" t="s">
         <v>153</v>
       </c>
       <c r="E70" s="46" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="30">
       <c r="B71" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C71" s="55"/>
       <c r="D71" t="s">
         <v>154</v>
       </c>
       <c r="E71" s="46" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="30">
       <c r="B72" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C72" s="56"/>
       <c r="D72" t="s">
+        <v>241</v>
+      </c>
+      <c r="E72" s="46" t="s">
         <v>244</v>
-      </c>
-      <c r="E72" s="46" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="30">
       <c r="B73" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C73" s="56"/>
       <c r="D73" t="s">
         <v>156</v>
       </c>
       <c r="E73" s="46" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:18">
       <c r="B74" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C74" s="57"/>
       <c r="D74" t="s">
         <v>157</v>
       </c>
       <c r="E74" s="46" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:18">
       <c r="B75" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C75" s="57"/>
       <c r="D75" t="s">
         <v>158</v>
       </c>
       <c r="E75" s="46" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="76" spans="1:18">
       <c r="B76" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C76" s="52"/>
       <c r="D76" t="s">
@@ -2637,7 +2637,7 @@
     </row>
     <row r="77" spans="1:18">
       <c r="B77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C77" s="52"/>
       <c r="D77" t="s">
@@ -2652,14 +2652,14 @@
     </row>
     <row r="78" spans="1:18">
       <c r="B78" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C78" s="53"/>
       <c r="D78" t="s">
+        <v>206</v>
+      </c>
+      <c r="E78" s="46" t="s">
         <v>207</v>
-      </c>
-      <c r="E78" s="46" t="s">
-        <v>208</v>
       </c>
       <c r="R78" t="s">
         <v>113</v>
@@ -2667,14 +2667,14 @@
     </row>
     <row r="79" spans="1:18">
       <c r="B79" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C79" s="53"/>
       <c r="D79" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E79" s="46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R79" t="s">
         <v>113</v>
@@ -2682,11 +2682,11 @@
     </row>
     <row r="80" spans="1:18">
       <c r="B80" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C80" s="54"/>
       <c r="E80" s="46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="R80" t="s">
         <v>113</v>
@@ -2694,10 +2694,10 @@
     </row>
     <row r="81" spans="4:5">
       <c r="D81" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E81" s="46" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="4:5">
@@ -2705,15 +2705,15 @@
         <v>137</v>
       </c>
       <c r="E82" s="46" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="4:5" ht="30">
       <c r="D83" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E83" s="46" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed cruise control / speed limiting indicator lamp from LED_FAULT_1 (alternator light) to LED_FAULT_3 (headlight retractor light). Changed the EVCU wiring diagram and spreadsheet to include wiring from LED_FAULT_3 to the headlight retractor light on the dash via a red-black wire and a diode.
</commit_message>
<xml_diff>
--- a/master/tritium/DCU wiring.xlsx
+++ b/master/tritium/DCU wiring.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="256">
   <si>
     <t>1A</t>
   </si>
@@ -622,12 +621,6 @@
     <t>Stress level gauge (pressure gauge), Gauge2, Joined to YEL-RED2 under dash</t>
   </si>
   <si>
-    <t>LED_FAULT_1, joined to WHT-BLK under dash, Alternator light (Inst cluster)</t>
-  </si>
-  <si>
-    <t>Not used. May be the one that's cut under dash. See BLU-ORG-SLV</t>
-  </si>
-  <si>
     <t>Fan switch. Switched to GND when fan on speed 2 or more</t>
   </si>
   <si>
@@ -776,6 +769,21 @@
   </si>
   <si>
     <t>Joined to RED-BLU under the dash, Powers IMUs in contactor boxes A2 and B2</t>
+  </si>
+  <si>
+    <t>no wire</t>
+  </si>
+  <si>
+    <t>LED_FAULT_1, joined to inst cluster WHT-BLK under dash, Alternator light (active low). Had to cut two tracks on back of inst cluster to separate from brake warning light and resistors.</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>LED_FAULT_3, cut under dash and joined via diode to inst cluster GRN-BLU. Headlight retractor light (active high).</t>
+  </si>
+  <si>
+    <t>The unused thin BLU_ORG at the ECU location is not connected to the thin BLU-ORG that is cut under the dash. I have no idea where either of these go..</t>
   </si>
 </sst>
 </file>
@@ -1360,9 +1368,9 @@
   <dimension ref="A1:R83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="750" topLeftCell="A48" activePane="bottomLeft"/>
+      <pane ySplit="750" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1377,7 +1385,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="46" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>128</v>
@@ -1389,7 +1397,7 @@
         <v>133</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>177</v>
@@ -1445,7 +1453,7 @@
         <v>164</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1462,7 +1470,7 @@
         <v>79</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -1479,7 +1487,7 @@
     </row>
     <row r="4" spans="1:18" ht="45">
       <c r="A4" s="46" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
@@ -1491,7 +1499,7 @@
         <v>151</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
@@ -1511,7 +1519,7 @@
         <v>79</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -1574,7 +1582,7 @@
         <v>79</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -1594,7 +1602,7 @@
         <v>79</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -1604,6 +1612,9 @@
       </c>
     </row>
     <row r="10" spans="1:18">
+      <c r="B10" t="s">
+        <v>251</v>
+      </c>
       <c r="C10" s="36"/>
       <c r="F10" t="s">
         <v>8</v>
@@ -1637,7 +1648,7 @@
         <v>79</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -1647,12 +1658,18 @@
       </c>
     </row>
     <row r="13" spans="1:18">
+      <c r="B13" t="s">
+        <v>251</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="F13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:18">
+      <c r="B14" t="s">
+        <v>251</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="F14" t="s">
         <v>12</v>
@@ -1701,7 +1718,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="30">
+    <row r="17" spans="1:16" ht="60">
       <c r="A17" s="46" t="s">
         <v>88</v>
       </c>
@@ -1715,7 +1732,7 @@
         <v>193</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>201</v>
+        <v>252</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -1749,7 +1766,7 @@
         <v>79</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
@@ -1758,7 +1775,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="30">
+    <row r="20" spans="1:16" ht="45">
       <c r="A20" s="46" t="s">
         <v>188</v>
       </c>
@@ -1769,19 +1786,22 @@
         <v>79</v>
       </c>
       <c r="E20" s="46" t="s">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:16">
+      <c r="B21" t="s">
+        <v>251</v>
+      </c>
       <c r="C21" s="36"/>
       <c r="F21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" ht="45">
       <c r="A22" s="46" t="s">
         <v>91</v>
       </c>
@@ -1790,6 +1810,12 @@
       </c>
       <c r="C22" s="18" t="s">
         <v>79</v>
+      </c>
+      <c r="D22" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>254</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
@@ -1806,10 +1832,10 @@
         <v>79</v>
       </c>
       <c r="D23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F23" t="s">
         <v>21</v>
@@ -1919,6 +1945,9 @@
       </c>
     </row>
     <row r="29" spans="1:16">
+      <c r="B29" t="s">
+        <v>251</v>
+      </c>
       <c r="C29" s="36"/>
       <c r="F29" t="s">
         <v>27</v>
@@ -1958,7 +1987,7 @@
         <v>79</v>
       </c>
       <c r="E31" s="46" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F31" t="s">
         <v>29</v>
@@ -1988,6 +2017,9 @@
       </c>
     </row>
     <row r="33" spans="1:15">
+      <c r="B33" t="s">
+        <v>251</v>
+      </c>
       <c r="C33" s="36"/>
       <c r="F33" t="s">
         <v>31</v>
@@ -2052,7 +2084,7 @@
         <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C37" s="29" t="s">
         <v>79</v>
@@ -2063,10 +2095,10 @@
     </row>
     <row r="38" spans="1:15" ht="30">
       <c r="A38" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>79</v>
@@ -2106,28 +2138,37 @@
         <v>79</v>
       </c>
       <c r="D40" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F40" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:15">
+      <c r="B41" t="s">
+        <v>251</v>
+      </c>
       <c r="C41" s="37"/>
       <c r="F41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:15">
+      <c r="B42" t="s">
+        <v>251</v>
+      </c>
       <c r="C42" s="35"/>
       <c r="F42" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:15">
+      <c r="B43" t="s">
+        <v>251</v>
+      </c>
       <c r="C43" s="38"/>
       <c r="F43" t="s">
         <v>41</v>
@@ -2164,7 +2205,7 @@
         <v>162</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F45" t="s">
         <v>43</v>
@@ -2184,7 +2225,7 @@
         <v>196</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F46" t="s">
         <v>60</v>
@@ -2228,6 +2269,9 @@
       </c>
     </row>
     <row r="49" spans="1:17">
+      <c r="B49" t="s">
+        <v>251</v>
+      </c>
       <c r="C49" s="37"/>
       <c r="F49" t="s">
         <v>62</v>
@@ -2248,7 +2292,7 @@
     </row>
     <row r="52" spans="1:17" ht="45">
       <c r="A52" s="46" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B52" t="s">
         <v>194</v>
@@ -2376,7 +2420,7 @@
         <v>79</v>
       </c>
       <c r="E59" s="46" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K59" t="s">
         <v>113</v>
@@ -2396,7 +2440,7 @@
         <v>79</v>
       </c>
       <c r="E60" s="46" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G60" t="s">
         <v>113</v>
@@ -2467,14 +2511,14 @@
     </row>
     <row r="64" spans="1:17" ht="30">
       <c r="A64" s="46" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B64" t="s">
         <v>175</v>
       </c>
       <c r="C64" s="33"/>
       <c r="E64" s="46" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="Q64" t="s">
         <v>113</v>
@@ -2482,14 +2526,14 @@
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="46" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B65" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C65" s="33"/>
       <c r="E65" s="46" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H65" t="s">
         <v>0</v>
@@ -2500,7 +2544,7 @@
     </row>
     <row r="66" spans="1:18" ht="30">
       <c r="A66" s="46" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B66" t="s">
         <v>189</v>
@@ -2509,7 +2553,7 @@
         <v>79</v>
       </c>
       <c r="E66" s="46" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H66" t="s">
         <v>23</v>
@@ -2517,16 +2561,16 @@
     </row>
     <row r="67" spans="1:18">
       <c r="A67" s="46" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B67" t="s">
+        <v>215</v>
+      </c>
+      <c r="C67" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="E67" s="46" t="s">
         <v>217</v>
-      </c>
-      <c r="C67" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="E67" s="46" t="s">
-        <v>219</v>
       </c>
       <c r="H67" t="s">
         <v>33</v>
@@ -2537,7 +2581,7 @@
         <v>149</v>
       </c>
       <c r="E68" s="46" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="69" spans="1:18">
@@ -2545,7 +2589,7 @@
         <v>150</v>
       </c>
       <c r="E69" s="46" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="70" spans="1:18">
@@ -2557,7 +2601,7 @@
         <v>153</v>
       </c>
       <c r="E70" s="46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="30">
@@ -2569,7 +2613,7 @@
         <v>154</v>
       </c>
       <c r="E71" s="46" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="30">
@@ -2578,10 +2622,10 @@
       </c>
       <c r="C72" s="56"/>
       <c r="D72" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E72" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="30">
@@ -2593,7 +2637,7 @@
         <v>156</v>
       </c>
       <c r="E73" s="46" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="74" spans="1:18">
@@ -2605,7 +2649,7 @@
         <v>157</v>
       </c>
       <c r="E74" s="46" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="75" spans="1:18">
@@ -2617,7 +2661,7 @@
         <v>158</v>
       </c>
       <c r="E75" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="76" spans="1:18">
@@ -2656,10 +2700,10 @@
       </c>
       <c r="C78" s="53"/>
       <c r="D78" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E78" s="46" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="R78" t="s">
         <v>113</v>
@@ -2671,10 +2715,10 @@
       </c>
       <c r="C79" s="53"/>
       <c r="D79" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E79" s="46" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="R79" t="s">
         <v>113</v>
@@ -2694,10 +2738,10 @@
     </row>
     <row r="81" spans="4:5">
       <c r="D81" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E81" s="46" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="4:5">
@@ -2705,15 +2749,15 @@
         <v>137</v>
       </c>
       <c r="E82" s="46" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="4:5" ht="30">
       <c r="D83" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E83" s="46" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>